<commit_message>
change comparator to LM311 on motherboard due to conflicting information in the datasheet of the old part, the LM331
</commit_message>
<xml_diff>
--- a/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
+++ b/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="800" windowWidth="14400" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="partlistKicker" localSheetId="0">Sheet1!$A$1:$F$127</definedName>
   </definedNames>
-  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1675,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added to the BOM
</commit_message>
<xml_diff>
--- a/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
+++ b/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="383">
   <si>
     <t>Partlist</t>
   </si>
@@ -386,9 +386,6 @@
     <t>CAP_COMP</t>
   </si>
   <si>
-    <t>LM331</t>
-  </si>
-  <si>
     <t>SOT23-5</t>
   </si>
   <si>
@@ -1100,9 +1097,6 @@
     <t>need to get a crimper?</t>
   </si>
   <si>
-    <t>296-6633-1-ND</t>
-  </si>
-  <si>
     <t>MCP6291T-E/OTCT-ND</t>
   </si>
   <si>
@@ -1182,6 +1176,18 @@
   </si>
   <si>
     <t>ATSAM3S4BA-AU-ND</t>
+  </si>
+  <si>
+    <t>LM311</t>
+  </si>
+  <si>
+    <t>SOIC8</t>
+  </si>
+  <si>
+    <t>gen5</t>
+  </si>
+  <si>
+    <t>MAKE SURE TO GET LEDs with small forward voltage. Must be able to drive with 3.3V</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1260,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1305,7 +1315,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1323,6 +1333,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1340,6 +1352,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1675,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1743,10 +1757,10 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1769,7 +1783,7 @@
         <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1792,7 +1806,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1815,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1841,7 +1855,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -1856,7 +1870,7 @@
         <v>19</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1864,7 +1878,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -1879,7 +1893,7 @@
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2522,67 +2536,65 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>114</v>
       </c>
       <c r="B49" t="s">
+        <v>379</v>
+      </c>
+      <c r="C49" t="s">
+        <v>380</v>
+      </c>
+      <c r="D49" t="s">
+        <v>381</v>
+      </c>
+      <c r="E49" t="s">
+        <v>116</v>
+      </c>
+      <c r="F49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>360</v>
+      </c>
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
         <v>115</v>
       </c>
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" t="s">
-        <v>117</v>
-      </c>
-      <c r="F49" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>362</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>118</v>
       </c>
-      <c r="C50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>119</v>
       </c>
-      <c r="E50" t="s">
-        <v>120</v>
-      </c>
       <c r="F50" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" t="s">
         <v>121</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>122</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>123</v>
-      </c>
-      <c r="E51" t="s">
-        <v>124</v>
       </c>
       <c r="F51" t="s">
         <v>19</v>
@@ -2590,13 +2602,16 @@
       <c r="H51">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
         <v>125</v>
-      </c>
-      <c r="B52" t="s">
-        <v>126</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -2605,90 +2620,90 @@
         <v>17</v>
       </c>
       <c r="E52" t="s">
+        <v>126</v>
+      </c>
+      <c r="F52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
         <v>127</v>
       </c>
-      <c r="F52" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="5" t="s">
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>131</v>
-      </c>
-      <c r="E53" t="s">
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
         <v>132</v>
       </c>
-      <c r="F53" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
         <v>133</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>134</v>
-      </c>
-      <c r="C54" t="s">
-        <v>135</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
       </c>
       <c r="E54" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B56" t="s">
         <v>25</v>
@@ -2700,18 +2715,18 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
+        <v>140</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
         <v>141</v>
-      </c>
-      <c r="F56" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>142</v>
       </c>
       <c r="B57" t="s">
         <v>25</v>
@@ -2723,30 +2738,30 @@
         <v>17</v>
       </c>
       <c r="E57" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F57" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>19</v>
@@ -2754,61 +2769,61 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F59" t="s">
         <v>19</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H59">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F60" t="s">
         <v>19</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
@@ -2817,28 +2832,28 @@
         <v>17</v>
       </c>
       <c r="E61" t="s">
+        <v>150</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="F61" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>19</v>
@@ -2848,19 +2863,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:9">
       <c r="A63" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>19</v>
@@ -2870,19 +2885,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="E64" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>19</v>
@@ -2891,7 +2906,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
@@ -2900,13 +2915,13 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F65" t="s">
         <v>19</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -2914,19 +2929,19 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>19</v>
@@ -2936,55 +2951,55 @@
         <v>4</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" t="s">
         <v>164</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>165</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>166</v>
       </c>
-      <c r="E67" t="s">
-        <v>167</v>
-      </c>
       <c r="F67" t="s">
         <v>19</v>
       </c>
       <c r="G67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
+        <v>167</v>
+      </c>
+      <c r="B68" t="s">
         <v>168</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>169</v>
-      </c>
-      <c r="C68" t="s">
-        <v>170</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F68" t="s">
         <v>19</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B69">
         <v>100</v>
@@ -2993,10 +3008,10 @@
         <v>805</v>
       </c>
       <c r="D69" t="s">
+        <v>172</v>
+      </c>
+      <c r="E69" t="s">
         <v>173</v>
-      </c>
-      <c r="E69" t="s">
-        <v>174</v>
       </c>
       <c r="F69" t="s">
         <v>19</v>
@@ -3004,7 +3019,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B70">
         <v>100</v>
@@ -3013,10 +3028,10 @@
         <v>805</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F70" t="s">
         <v>19</v>
@@ -3024,19 +3039,19 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" t="s">
         <v>177</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71">
+        <v>805</v>
+      </c>
+      <c r="D71" t="s">
         <v>178</v>
       </c>
-      <c r="C71">
-        <v>805</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>179</v>
-      </c>
-      <c r="E71" t="s">
-        <v>180</v>
       </c>
       <c r="F71" t="s">
         <v>19</v>
@@ -3044,19 +3059,19 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" t="s">
         <v>181</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72">
+        <v>805</v>
+      </c>
+      <c r="D72" t="s">
+        <v>178</v>
+      </c>
+      <c r="E72" t="s">
         <v>182</v>
-      </c>
-      <c r="C72">
-        <v>805</v>
-      </c>
-      <c r="D72" t="s">
-        <v>179</v>
-      </c>
-      <c r="E72" t="s">
-        <v>183</v>
       </c>
       <c r="F72" t="s">
         <v>19</v>
@@ -3064,19 +3079,19 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73">
+        <v>805</v>
+      </c>
+      <c r="D73" t="s">
+        <v>178</v>
+      </c>
+      <c r="E73" t="s">
         <v>184</v>
-      </c>
-      <c r="B73" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73">
-        <v>805</v>
-      </c>
-      <c r="D73" t="s">
-        <v>179</v>
-      </c>
-      <c r="E73" t="s">
-        <v>185</v>
       </c>
       <c r="F73" t="s">
         <v>19</v>
@@ -3084,19 +3099,19 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
+        <v>185</v>
+      </c>
+      <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74">
+        <v>805</v>
+      </c>
+      <c r="D74" t="s">
+        <v>178</v>
+      </c>
+      <c r="E74" t="s">
         <v>186</v>
-      </c>
-      <c r="B74" t="s">
-        <v>182</v>
-      </c>
-      <c r="C74">
-        <v>805</v>
-      </c>
-      <c r="D74" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" t="s">
-        <v>187</v>
       </c>
       <c r="F74" t="s">
         <v>19</v>
@@ -3104,19 +3119,19 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
+        <v>187</v>
+      </c>
+      <c r="B75" t="s">
         <v>188</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75">
+        <v>805</v>
+      </c>
+      <c r="D75" t="s">
+        <v>178</v>
+      </c>
+      <c r="E75" t="s">
         <v>189</v>
-      </c>
-      <c r="C75">
-        <v>805</v>
-      </c>
-      <c r="D75" t="s">
-        <v>179</v>
-      </c>
-      <c r="E75" t="s">
-        <v>190</v>
       </c>
       <c r="F75" t="s">
         <v>19</v>
@@ -3124,19 +3139,19 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76">
+        <v>805</v>
+      </c>
+      <c r="D76" t="s">
+        <v>178</v>
+      </c>
+      <c r="E76" t="s">
         <v>191</v>
-      </c>
-      <c r="B76" t="s">
-        <v>182</v>
-      </c>
-      <c r="C76">
-        <v>805</v>
-      </c>
-      <c r="D76" t="s">
-        <v>179</v>
-      </c>
-      <c r="E76" t="s">
-        <v>192</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
@@ -3144,19 +3159,19 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
+        <v>192</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77">
+        <v>805</v>
+      </c>
+      <c r="D77" t="s">
+        <v>178</v>
+      </c>
+      <c r="E77" t="s">
         <v>193</v>
-      </c>
-      <c r="B77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77">
-        <v>805</v>
-      </c>
-      <c r="D77" t="s">
-        <v>179</v>
-      </c>
-      <c r="E77" t="s">
-        <v>194</v>
       </c>
       <c r="F77" t="s">
         <v>19</v>
@@ -3164,19 +3179,19 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
+        <v>194</v>
+      </c>
+      <c r="B78" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78">
+        <v>805</v>
+      </c>
+      <c r="D78" t="s">
+        <v>178</v>
+      </c>
+      <c r="E78" t="s">
         <v>195</v>
-      </c>
-      <c r="B78" t="s">
-        <v>182</v>
-      </c>
-      <c r="C78">
-        <v>805</v>
-      </c>
-      <c r="D78" t="s">
-        <v>179</v>
-      </c>
-      <c r="E78" t="s">
-        <v>196</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -3184,19 +3199,19 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
+        <v>196</v>
+      </c>
+      <c r="B79" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79">
+        <v>805</v>
+      </c>
+      <c r="D79" t="s">
+        <v>178</v>
+      </c>
+      <c r="E79" t="s">
         <v>197</v>
-      </c>
-      <c r="B79" t="s">
-        <v>182</v>
-      </c>
-      <c r="C79">
-        <v>805</v>
-      </c>
-      <c r="D79" t="s">
-        <v>179</v>
-      </c>
-      <c r="E79" t="s">
-        <v>198</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -3204,19 +3219,19 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80">
+        <v>805</v>
+      </c>
+      <c r="D80" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" t="s">
         <v>199</v>
-      </c>
-      <c r="B80" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80">
-        <v>805</v>
-      </c>
-      <c r="D80" t="s">
-        <v>179</v>
-      </c>
-      <c r="E80" t="s">
-        <v>200</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
@@ -3224,19 +3239,19 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" t="s">
         <v>201</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81">
+        <v>805</v>
+      </c>
+      <c r="D81" t="s">
+        <v>178</v>
+      </c>
+      <c r="E81" t="s">
         <v>202</v>
-      </c>
-      <c r="C81">
-        <v>805</v>
-      </c>
-      <c r="D81" t="s">
-        <v>179</v>
-      </c>
-      <c r="E81" t="s">
-        <v>203</v>
       </c>
       <c r="F81" t="s">
         <v>19</v>
@@ -3244,19 +3259,19 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
+        <v>203</v>
+      </c>
+      <c r="B82" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82">
+        <v>805</v>
+      </c>
+      <c r="D82" t="s">
+        <v>172</v>
+      </c>
+      <c r="E82" t="s">
         <v>204</v>
-      </c>
-      <c r="B82" t="s">
-        <v>189</v>
-      </c>
-      <c r="C82">
-        <v>805</v>
-      </c>
-      <c r="D82" t="s">
-        <v>173</v>
-      </c>
-      <c r="E82" t="s">
-        <v>205</v>
       </c>
       <c r="F82" t="s">
         <v>19</v>
@@ -3264,19 +3279,19 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" t="s">
         <v>206</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83">
+        <v>805</v>
+      </c>
+      <c r="D83" t="s">
+        <v>172</v>
+      </c>
+      <c r="E83" t="s">
         <v>207</v>
-      </c>
-      <c r="C83">
-        <v>805</v>
-      </c>
-      <c r="D83" t="s">
-        <v>173</v>
-      </c>
-      <c r="E83" t="s">
-        <v>208</v>
       </c>
       <c r="F83" t="s">
         <v>19</v>
@@ -3284,19 +3299,19 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
+        <v>208</v>
+      </c>
+      <c r="B84" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84">
+        <v>805</v>
+      </c>
+      <c r="D84" t="s">
+        <v>178</v>
+      </c>
+      <c r="E84" t="s">
         <v>209</v>
-      </c>
-      <c r="B84" t="s">
-        <v>182</v>
-      </c>
-      <c r="C84">
-        <v>805</v>
-      </c>
-      <c r="D84" t="s">
-        <v>179</v>
-      </c>
-      <c r="E84" t="s">
-        <v>210</v>
       </c>
       <c r="F84" t="s">
         <v>19</v>
@@ -3304,19 +3319,19 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85" t="s">
         <v>211</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85">
+        <v>805</v>
+      </c>
+      <c r="D85" t="s">
+        <v>178</v>
+      </c>
+      <c r="E85" t="s">
         <v>212</v>
-      </c>
-      <c r="C85">
-        <v>805</v>
-      </c>
-      <c r="D85" t="s">
-        <v>179</v>
-      </c>
-      <c r="E85" t="s">
-        <v>213</v>
       </c>
       <c r="F85" t="s">
         <v>19</v>
@@ -3324,19 +3339,19 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
+        <v>213</v>
+      </c>
+      <c r="B86" t="s">
         <v>214</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86">
+        <v>805</v>
+      </c>
+      <c r="D86" t="s">
+        <v>178</v>
+      </c>
+      <c r="E86" t="s">
         <v>215</v>
-      </c>
-      <c r="C86">
-        <v>805</v>
-      </c>
-      <c r="D86" t="s">
-        <v>179</v>
-      </c>
-      <c r="E86" t="s">
-        <v>216</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
@@ -3344,7 +3359,7 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B87">
         <v>20</v>
@@ -3353,10 +3368,10 @@
         <v>805</v>
       </c>
       <c r="D87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
         <v>19</v>
@@ -3364,7 +3379,7 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B88">
         <v>100</v>
@@ -3373,10 +3388,10 @@
         <v>805</v>
       </c>
       <c r="D88" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E88" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F88" t="s">
         <v>19</v>
@@ -3384,19 +3399,19 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
+        <v>220</v>
+      </c>
+      <c r="B89" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89">
+        <v>805</v>
+      </c>
+      <c r="D89" t="s">
+        <v>178</v>
+      </c>
+      <c r="E89" t="s">
         <v>221</v>
-      </c>
-      <c r="B89" t="s">
-        <v>182</v>
-      </c>
-      <c r="C89">
-        <v>805</v>
-      </c>
-      <c r="D89" t="s">
-        <v>179</v>
-      </c>
-      <c r="E89" t="s">
-        <v>222</v>
       </c>
       <c r="F89" t="s">
         <v>19</v>
@@ -3404,19 +3419,19 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90">
+        <v>805</v>
+      </c>
+      <c r="D90" t="s">
+        <v>178</v>
+      </c>
+      <c r="E90" t="s">
         <v>223</v>
-      </c>
-      <c r="B90" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90">
-        <v>805</v>
-      </c>
-      <c r="D90" t="s">
-        <v>179</v>
-      </c>
-      <c r="E90" t="s">
-        <v>224</v>
       </c>
       <c r="F90" t="s">
         <v>19</v>
@@ -3424,19 +3439,19 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
         <v>225</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91">
+        <v>805</v>
+      </c>
+      <c r="D91" t="s">
+        <v>178</v>
+      </c>
+      <c r="E91" t="s">
         <v>226</v>
-      </c>
-      <c r="C91">
-        <v>805</v>
-      </c>
-      <c r="D91" t="s">
-        <v>179</v>
-      </c>
-      <c r="E91" t="s">
-        <v>227</v>
       </c>
       <c r="F91" t="s">
         <v>19</v>
@@ -3444,19 +3459,19 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" t="s">
         <v>228</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92">
+        <v>805</v>
+      </c>
+      <c r="D92" t="s">
+        <v>178</v>
+      </c>
+      <c r="E92" t="s">
         <v>229</v>
-      </c>
-      <c r="C92">
-        <v>805</v>
-      </c>
-      <c r="D92" t="s">
-        <v>179</v>
-      </c>
-      <c r="E92" t="s">
-        <v>230</v>
       </c>
       <c r="F92" t="s">
         <v>19</v>
@@ -3464,7 +3479,7 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B93">
         <v>200</v>
@@ -3473,10 +3488,10 @@
         <v>805</v>
       </c>
       <c r="D93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F93" t="s">
         <v>19</v>
@@ -3484,7 +3499,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B94">
         <v>300</v>
@@ -3493,10 +3508,10 @@
         <v>805</v>
       </c>
       <c r="D94" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E94" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F94" t="s">
         <v>19</v>
@@ -3504,19 +3519,19 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
+        <v>234</v>
+      </c>
+      <c r="B95" t="s">
         <v>235</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95">
+        <v>805</v>
+      </c>
+      <c r="D95" t="s">
+        <v>172</v>
+      </c>
+      <c r="E95" t="s">
         <v>236</v>
-      </c>
-      <c r="C95">
-        <v>805</v>
-      </c>
-      <c r="D95" t="s">
-        <v>173</v>
-      </c>
-      <c r="E95" t="s">
-        <v>237</v>
       </c>
       <c r="F95" t="s">
         <v>19</v>
@@ -3524,19 +3539,19 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
+        <v>237</v>
+      </c>
+      <c r="B96" t="s">
+        <v>235</v>
+      </c>
+      <c r="C96">
+        <v>805</v>
+      </c>
+      <c r="D96" t="s">
+        <v>172</v>
+      </c>
+      <c r="E96" t="s">
         <v>238</v>
-      </c>
-      <c r="B96" t="s">
-        <v>236</v>
-      </c>
-      <c r="C96">
-        <v>805</v>
-      </c>
-      <c r="D96" t="s">
-        <v>173</v>
-      </c>
-      <c r="E96" t="s">
-        <v>239</v>
       </c>
       <c r="F96" t="s">
         <v>19</v>
@@ -3544,19 +3559,19 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>239</v>
+      </c>
+      <c r="B97" t="s">
         <v>240</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97">
+        <v>805</v>
+      </c>
+      <c r="D97" t="s">
+        <v>178</v>
+      </c>
+      <c r="E97" t="s">
         <v>241</v>
-      </c>
-      <c r="C97">
-        <v>805</v>
-      </c>
-      <c r="D97" t="s">
-        <v>179</v>
-      </c>
-      <c r="E97" t="s">
-        <v>242</v>
       </c>
       <c r="F97" t="s">
         <v>19</v>
@@ -3564,19 +3579,19 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
+        <v>242</v>
+      </c>
+      <c r="B98" t="s">
+        <v>235</v>
+      </c>
+      <c r="C98">
+        <v>805</v>
+      </c>
+      <c r="D98" t="s">
+        <v>172</v>
+      </c>
+      <c r="E98" t="s">
         <v>243</v>
-      </c>
-      <c r="B98" t="s">
-        <v>236</v>
-      </c>
-      <c r="C98">
-        <v>805</v>
-      </c>
-      <c r="D98" t="s">
-        <v>173</v>
-      </c>
-      <c r="E98" t="s">
-        <v>244</v>
       </c>
       <c r="F98" t="s">
         <v>19</v>
@@ -3584,19 +3599,19 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
+        <v>244</v>
+      </c>
+      <c r="B99" t="s">
         <v>245</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99">
+        <v>805</v>
+      </c>
+      <c r="D99" t="s">
+        <v>178</v>
+      </c>
+      <c r="E99" t="s">
         <v>246</v>
-      </c>
-      <c r="C99">
-        <v>805</v>
-      </c>
-      <c r="D99" t="s">
-        <v>179</v>
-      </c>
-      <c r="E99" t="s">
-        <v>247</v>
       </c>
       <c r="F99" t="s">
         <v>19</v>
@@ -3604,19 +3619,19 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
+        <v>247</v>
+      </c>
+      <c r="B100" t="s">
+        <v>235</v>
+      </c>
+      <c r="C100">
+        <v>805</v>
+      </c>
+      <c r="D100" t="s">
+        <v>172</v>
+      </c>
+      <c r="E100" t="s">
         <v>248</v>
-      </c>
-      <c r="B100" t="s">
-        <v>236</v>
-      </c>
-      <c r="C100">
-        <v>805</v>
-      </c>
-      <c r="D100" t="s">
-        <v>173</v>
-      </c>
-      <c r="E100" t="s">
-        <v>249</v>
       </c>
       <c r="F100" t="s">
         <v>19</v>
@@ -3624,19 +3639,19 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
+        <v>249</v>
+      </c>
+      <c r="B101" t="s">
+        <v>235</v>
+      </c>
+      <c r="C101">
+        <v>805</v>
+      </c>
+      <c r="D101" t="s">
+        <v>172</v>
+      </c>
+      <c r="E101" t="s">
         <v>250</v>
-      </c>
-      <c r="B101" t="s">
-        <v>236</v>
-      </c>
-      <c r="C101">
-        <v>805</v>
-      </c>
-      <c r="D101" t="s">
-        <v>173</v>
-      </c>
-      <c r="E101" t="s">
-        <v>251</v>
       </c>
       <c r="F101" t="s">
         <v>19</v>
@@ -3644,19 +3659,19 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
+        <v>251</v>
+      </c>
+      <c r="B102" t="s">
+        <v>206</v>
+      </c>
+      <c r="C102">
+        <v>805</v>
+      </c>
+      <c r="D102" t="s">
+        <v>172</v>
+      </c>
+      <c r="E102" t="s">
         <v>252</v>
-      </c>
-      <c r="B102" t="s">
-        <v>207</v>
-      </c>
-      <c r="C102">
-        <v>805</v>
-      </c>
-      <c r="D102" t="s">
-        <v>173</v>
-      </c>
-      <c r="E102" t="s">
-        <v>253</v>
       </c>
       <c r="F102" t="s">
         <v>19</v>
@@ -3664,19 +3679,19 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103" t="s">
         <v>254</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103">
+        <v>805</v>
+      </c>
+      <c r="D103" t="s">
+        <v>172</v>
+      </c>
+      <c r="E103" t="s">
         <v>255</v>
-      </c>
-      <c r="C103">
-        <v>805</v>
-      </c>
-      <c r="D103" t="s">
-        <v>173</v>
-      </c>
-      <c r="E103" t="s">
-        <v>256</v>
       </c>
       <c r="F103" t="s">
         <v>19</v>
@@ -3684,19 +3699,19 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
+        <v>256</v>
+      </c>
+      <c r="B104" t="s">
+        <v>254</v>
+      </c>
+      <c r="C104">
+        <v>805</v>
+      </c>
+      <c r="D104" t="s">
+        <v>172</v>
+      </c>
+      <c r="E104" t="s">
         <v>257</v>
-      </c>
-      <c r="B104" t="s">
-        <v>255</v>
-      </c>
-      <c r="C104">
-        <v>805</v>
-      </c>
-      <c r="D104" t="s">
-        <v>173</v>
-      </c>
-      <c r="E104" t="s">
-        <v>258</v>
       </c>
       <c r="F104" t="s">
         <v>19</v>
@@ -3704,19 +3719,19 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
+        <v>258</v>
+      </c>
+      <c r="B105" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105">
+        <v>805</v>
+      </c>
+      <c r="D105" t="s">
+        <v>178</v>
+      </c>
+      <c r="E105" t="s">
         <v>259</v>
-      </c>
-      <c r="B105" t="s">
-        <v>182</v>
-      </c>
-      <c r="C105">
-        <v>805</v>
-      </c>
-      <c r="D105" t="s">
-        <v>179</v>
-      </c>
-      <c r="E105" t="s">
-        <v>260</v>
       </c>
       <c r="F105" t="s">
         <v>19</v>
@@ -3724,19 +3739,19 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
+        <v>260</v>
+      </c>
+      <c r="B106" t="s">
         <v>261</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106">
+        <v>805</v>
+      </c>
+      <c r="D106" t="s">
+        <v>178</v>
+      </c>
+      <c r="E106" t="s">
         <v>262</v>
-      </c>
-      <c r="C106">
-        <v>805</v>
-      </c>
-      <c r="D106" t="s">
-        <v>179</v>
-      </c>
-      <c r="E106" t="s">
-        <v>263</v>
       </c>
       <c r="F106" t="s">
         <v>19</v>
@@ -3744,19 +3759,19 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C107">
+        <v>805</v>
+      </c>
+      <c r="D107" t="s">
+        <v>178</v>
+      </c>
+      <c r="E107" t="s">
         <v>264</v>
-      </c>
-      <c r="B107" t="s">
-        <v>189</v>
-      </c>
-      <c r="C107">
-        <v>805</v>
-      </c>
-      <c r="D107" t="s">
-        <v>179</v>
-      </c>
-      <c r="E107" t="s">
-        <v>265</v>
       </c>
       <c r="F107" t="s">
         <v>19</v>
@@ -3764,19 +3779,19 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
+        <v>265</v>
+      </c>
+      <c r="B108" t="s">
+        <v>261</v>
+      </c>
+      <c r="C108">
+        <v>805</v>
+      </c>
+      <c r="D108" t="s">
+        <v>178</v>
+      </c>
+      <c r="E108" t="s">
         <v>266</v>
-      </c>
-      <c r="B108" t="s">
-        <v>262</v>
-      </c>
-      <c r="C108">
-        <v>805</v>
-      </c>
-      <c r="D108" t="s">
-        <v>179</v>
-      </c>
-      <c r="E108" t="s">
-        <v>267</v>
       </c>
       <c r="F108" t="s">
         <v>19</v>
@@ -3784,19 +3799,19 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
+        <v>267</v>
+      </c>
+      <c r="B109" t="s">
         <v>268</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109">
+        <v>805</v>
+      </c>
+      <c r="D109" t="s">
+        <v>178</v>
+      </c>
+      <c r="E109" t="s">
         <v>269</v>
-      </c>
-      <c r="C109">
-        <v>805</v>
-      </c>
-      <c r="D109" t="s">
-        <v>179</v>
-      </c>
-      <c r="E109" t="s">
-        <v>270</v>
       </c>
       <c r="F109" t="s">
         <v>19</v>
@@ -3804,19 +3819,19 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>270</v>
+      </c>
+      <c r="B110" t="s">
+        <v>181</v>
+      </c>
+      <c r="C110">
+        <v>805</v>
+      </c>
+      <c r="D110" t="s">
+        <v>178</v>
+      </c>
+      <c r="E110" t="s">
         <v>271</v>
-      </c>
-      <c r="B110" t="s">
-        <v>182</v>
-      </c>
-      <c r="C110">
-        <v>805</v>
-      </c>
-      <c r="D110" t="s">
-        <v>179</v>
-      </c>
-      <c r="E110" t="s">
-        <v>272</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
@@ -3824,19 +3839,19 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
+        <v>272</v>
+      </c>
+      <c r="B111" t="s">
         <v>273</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111">
+        <v>805</v>
+      </c>
+      <c r="D111" t="s">
+        <v>178</v>
+      </c>
+      <c r="E111" t="s">
         <v>274</v>
-      </c>
-      <c r="C111">
-        <v>805</v>
-      </c>
-      <c r="D111" t="s">
-        <v>179</v>
-      </c>
-      <c r="E111" t="s">
-        <v>275</v>
       </c>
       <c r="F111" t="s">
         <v>19</v>
@@ -3844,19 +3859,19 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
+        <v>275</v>
+      </c>
+      <c r="B112" t="s">
         <v>276</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>277</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
+        <v>178</v>
+      </c>
+      <c r="E112" t="s">
         <v>278</v>
-      </c>
-      <c r="D112" t="s">
-        <v>179</v>
-      </c>
-      <c r="E112" t="s">
-        <v>279</v>
       </c>
       <c r="F112" t="s">
         <v>19</v>
@@ -3864,19 +3879,19 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
+        <v>279</v>
+      </c>
+      <c r="B113" t="s">
         <v>280</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113">
+        <v>805</v>
+      </c>
+      <c r="D113" t="s">
+        <v>178</v>
+      </c>
+      <c r="E113" t="s">
         <v>281</v>
-      </c>
-      <c r="C113">
-        <v>805</v>
-      </c>
-      <c r="D113" t="s">
-        <v>179</v>
-      </c>
-      <c r="E113" t="s">
-        <v>282</v>
       </c>
       <c r="F113" t="s">
         <v>19</v>
@@ -3884,25 +3899,25 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
+        <v>282</v>
+      </c>
+      <c r="B114" t="s">
+        <v>367</v>
+      </c>
+      <c r="C114" t="s">
+        <v>115</v>
+      </c>
+      <c r="D114" t="s">
+        <v>130</v>
+      </c>
+      <c r="E114" t="s">
         <v>283</v>
       </c>
-      <c r="B114" t="s">
-        <v>369</v>
-      </c>
-      <c r="C114" t="s">
-        <v>116</v>
-      </c>
-      <c r="D114" t="s">
-        <v>131</v>
-      </c>
-      <c r="E114" t="s">
-        <v>284</v>
-      </c>
       <c r="F114" t="s">
         <v>19</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H114">
         <v>2</v>
@@ -3910,134 +3925,134 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
+        <v>284</v>
+      </c>
+      <c r="B115" t="s">
         <v>285</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>286</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>287</v>
       </c>
-      <c r="D115" t="s">
+      <c r="E115" t="s">
         <v>288</v>
       </c>
-      <c r="E115" t="s">
-        <v>289</v>
-      </c>
       <c r="F115" t="s">
         <v>19</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
+        <v>289</v>
+      </c>
+      <c r="B116" t="s">
         <v>290</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>291</v>
-      </c>
-      <c r="C116" t="s">
-        <v>292</v>
       </c>
       <c r="D116" t="s">
         <v>17</v>
       </c>
       <c r="E116" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F116" t="s">
         <v>19</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
+        <v>293</v>
+      </c>
+      <c r="B117" t="s">
         <v>294</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>295</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
+        <v>287</v>
+      </c>
+      <c r="E117" t="s">
         <v>296</v>
       </c>
-      <c r="D117" t="s">
-        <v>288</v>
-      </c>
-      <c r="E117" t="s">
-        <v>297</v>
-      </c>
       <c r="F117" t="s">
         <v>19</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
+        <v>297</v>
+      </c>
+      <c r="B118" t="s">
         <v>298</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>299</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
+        <v>287</v>
+      </c>
+      <c r="E118" t="s">
         <v>300</v>
       </c>
-      <c r="D118" t="s">
-        <v>288</v>
-      </c>
-      <c r="E118" t="s">
-        <v>301</v>
-      </c>
       <c r="F118" t="s">
         <v>19</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
+        <v>301</v>
+      </c>
+      <c r="B119" t="s">
         <v>302</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>303</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
+        <v>287</v>
+      </c>
+      <c r="E119" t="s">
         <v>304</v>
       </c>
-      <c r="D119" t="s">
-        <v>288</v>
-      </c>
-      <c r="E119" t="s">
-        <v>305</v>
-      </c>
       <c r="F119" t="s">
         <v>19</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B120" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>19</v>
@@ -4048,33 +4063,33 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
+        <v>309</v>
+      </c>
+      <c r="B121" t="s">
         <v>310</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
+        <v>303</v>
+      </c>
+      <c r="D121" t="s">
+        <v>287</v>
+      </c>
+      <c r="E121" t="s">
         <v>311</v>
       </c>
-      <c r="C121" t="s">
-        <v>304</v>
-      </c>
-      <c r="D121" t="s">
-        <v>288</v>
-      </c>
-      <c r="E121" t="s">
-        <v>312</v>
-      </c>
       <c r="F121" t="s">
         <v>19</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B122" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="C122" s="3">
         <v>805</v>
@@ -4083,7 +4098,7 @@
         <v>17</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F122" s="3" t="s">
         <v>19</v>
@@ -4091,122 +4106,122 @@
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
+        <v>315</v>
+      </c>
+      <c r="B123" t="s">
         <v>316</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>317</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>318</v>
       </c>
-      <c r="D123" t="s">
+      <c r="E123" t="s">
         <v>319</v>
       </c>
-      <c r="E123" t="s">
-        <v>320</v>
-      </c>
       <c r="F123" t="s">
         <v>19</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
+        <v>320</v>
+      </c>
+      <c r="B124" t="s">
         <v>321</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>322</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
+        <v>318</v>
+      </c>
+      <c r="E124" t="s">
         <v>323</v>
       </c>
-      <c r="D124" t="s">
-        <v>319</v>
-      </c>
-      <c r="E124" t="s">
-        <v>324</v>
-      </c>
       <c r="F124" t="s">
         <v>19</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
+        <v>324</v>
+      </c>
+      <c r="B125" t="s">
         <v>325</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>326</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" t="s">
+        <v>318</v>
+      </c>
+      <c r="E125" t="s">
         <v>327</v>
       </c>
-      <c r="D125" t="s">
-        <v>319</v>
-      </c>
-      <c r="E125" t="s">
-        <v>328</v>
-      </c>
       <c r="F125" t="s">
         <v>19</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
+        <v>328</v>
+      </c>
+      <c r="B126" t="s">
         <v>329</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>330</v>
-      </c>
-      <c r="C126" t="s">
-        <v>331</v>
       </c>
       <c r="D126" t="s">
         <v>17</v>
       </c>
       <c r="E126" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F126" t="s">
         <v>19</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
+        <v>332</v>
+      </c>
+      <c r="B127" t="s">
         <v>333</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>334</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>335</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>336</v>
       </c>
-      <c r="E127" t="s">
-        <v>337</v>
-      </c>
       <c r="F127" t="s">
         <v>19</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="6"/>
@@ -4214,11 +4229,11 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pullups to the motorboard, and did DRC checking
</commit_message>
<xml_diff>
--- a/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
+++ b/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="0" windowWidth="21100" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="-20" windowWidth="14400" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="partlistKicker" localSheetId="0">Sheet1!$A$1:$F$78</definedName>
+    <definedName name="partlistKicker" localSheetId="0">Sheet1!$A$1:$F$69</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -39,31 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="315">
-  <si>
-    <t>Partlist</t>
-  </si>
-  <si>
-    <t>Exported from</t>
-  </si>
-  <si>
-    <t>KickerBoard.brd at</t>
-  </si>
-  <si>
-    <t>EAGLE Version</t>
-  </si>
-  <si>
-    <t>7.4.0 Copyright (c)</t>
-  </si>
-  <si>
-    <t>1988-2015 CadSoft</t>
-  </si>
-  <si>
-    <t>Assembly varia</t>
-  </si>
-  <si>
-    <t>nt:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="308">
   <si>
     <t>Part</t>
   </si>
@@ -984,6 +960,9 @@
   </si>
   <si>
     <t>we need a crimper?</t>
+  </si>
+  <si>
+    <t>WM10943CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1035,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1101,8 +1080,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1123,9 +1107,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1137,7 +1118,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1161,6 +1142,11 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1514,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1534,2140 +1520,2108 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I33" si="0">10*H2</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="12">
-        <v>42682.398611111108</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="11">
+        <v>805</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>10*H7*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>265</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1206</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11">
+        <v>805</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>213</v>
-      </c>
-      <c r="H9" t="s">
-        <v>229</v>
-      </c>
-      <c r="I9" t="s">
-        <v>313</v>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>249</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>214</v>
+        <v>269</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <f>10*H11</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="11">
+        <v>805</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f>10*H12*2</f>
         <v>20</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <f>10*H12</f>
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="11">
+        <v>805</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>216</v>
+        <v>271</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <f>10*H13</f>
-        <v>10</v>
+        <f>10*H13*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>248</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1206</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>221</v>
+        <v>268</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <f>10*H14</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
+      <c r="C15" s="11">
+        <v>805</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>218</v>
+        <v>267</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <f>10*H15</f>
-        <v>10</v>
+        <f>10*H15*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>42</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C16" s="11">
         <v>805</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>311</v>
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
-        <f>10*H16</f>
-        <v>10</v>
+        <f>10*H16*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>254</v>
+        <v>45</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C17" s="11">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>307</v>
+        <v>11</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <f>10*H17</f>
+        <f>10*H17*2</f>
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C18" s="11">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>308</v>
+        <v>11</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="I18">
-        <f>10*H18</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C19" s="11">
         <v>805</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>272</v>
+        <v>11</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>302</v>
       </c>
       <c r="H19">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <f>10*H19</f>
-        <v>120</v>
+        <f>10*H19*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>257</v>
+        <v>53</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>40</v>
+        <v>244</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>245</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>277</v>
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <f>10*H20</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="11">
-        <v>805</v>
+        <v>56</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>278</v>
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <f>10*H21</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="11">
-        <v>805</v>
+        <v>59</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>279</v>
+        <v>11</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>297</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I22">
-        <f>10*H22</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>63</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="11">
-        <v>1206</v>
+        <v>64</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>276</v>
+        <v>11</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <f>10*H23</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>274</v>
+        <v>66</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="11">
-        <v>805</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>275</v>
+        <v>67</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <f>10*H24</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="11">
-        <v>805</v>
+        <v>72</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>280</v>
+        <v>214</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
-        <f>10*H25</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="11">
-        <v>805</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>281</v>
+      <c r="A26" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26">
-        <f>10*H26</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>260</v>
+        <v>78</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="11">
-        <v>805</v>
+        <v>17</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>309</v>
+        <v>11</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H28" s="2">
         <v>2</v>
       </c>
-      <c r="I27">
-        <f>10*H27</f>
+      <c r="I28">
+        <f t="shared" si="0"/>
         <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="11">
-        <v>805</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f>10*H28</f>
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>252</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>253</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>306</v>
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29">
-        <f>10*H29</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>64</v>
+        <v>216</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>227</v>
+        <v>11</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I30">
-        <f>10*H30</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>305</v>
+        <v>11</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="H31">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <f>10*H31</f>
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>228</v>
+      <c r="A32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I32">
-        <f>10*H32</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>230</v>
-      </c>
+      <c r="A33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="2"/>
       <c r="H33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I33">
-        <f>10*H33</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <f>10*H34</f>
-        <v>10</v>
+        <f t="shared" ref="I34:I65" si="1">10*H34</f>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>236</v>
+        <v>96</v>
       </c>
       <c r="B35" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>216</v>
+        <v>11</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I35">
-        <f>10*H35</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="F36" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <f>10*H36</f>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
         <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="H37" s="2">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <f>10*H37</f>
-        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>234</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>81</v>
+        <v>253</v>
+      </c>
+      <c r="B38" s="9">
+        <v>100</v>
+      </c>
+      <c r="C38" s="11">
+        <v>805</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F38" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>217</v>
+        <v>274</v>
       </c>
       <c r="H38">
         <v>3</v>
       </c>
       <c r="I38">
-        <f>10*H38</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>234</v>
+        <v>108</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>81</v>
+        <v>109</v>
+      </c>
+      <c r="C39" s="11">
+        <v>805</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>222</v>
+        <v>11</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>288</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <f>10*H39</f>
-        <v>30</v>
+        <f>10*H39*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>16</v>
+        <v>254</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="11">
+        <v>805</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="F40" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>232</v>
+        <v>11</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I40">
-        <f>10*H40</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>269</v>
+      <c r="A41" t="s">
+        <v>260</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="11">
+        <v>805</v>
+      </c>
+      <c r="D41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="H41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <f>10*H41</f>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="2"/>
+      <c r="A42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="11">
+        <v>805</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="H42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I42">
-        <f>10*H42</f>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>238</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>16</v>
+        <v>257</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="11">
+        <v>805</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F43" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="H43">
         <v>3</v>
       </c>
       <c r="I43">
-        <f>10*H43</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>270</v>
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="11">
+        <v>805</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I44">
-        <f>10*H44</f>
-        <v>40</v>
+        <f>10*H44*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>107</v>
+        <v>122</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="11">
+        <v>805</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="F45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>312</v>
+        <v>11</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <f>10*H45</f>
-        <v>10</v>
+        <f>10*H45*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="9">
+        <v>20</v>
+      </c>
+      <c r="C46" s="11">
+        <v>805</v>
+      </c>
+      <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
       <c r="E46" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="F46" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <f>10*H46</f>
-        <v>10</v>
+        <f>10*H46*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>261</v>
-      </c>
-      <c r="B47" s="9">
-        <v>100</v>
+        <v>127</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="C47" s="11">
         <v>805</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="F47" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>282</v>
+        <v>11</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>289</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <f>10*H47</f>
-        <v>30</v>
+        <f>10*H47*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C48" s="11">
         <v>805</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E48" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="F48" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>296</v>
+        <v>11</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <f>10*H48</f>
-        <v>10</v>
+        <f>10*H48*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>262</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>120</v>
+        <v>133</v>
+      </c>
+      <c r="B49" s="9">
+        <v>200</v>
       </c>
       <c r="C49" s="11">
         <v>805</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F49" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>283</v>
+        <v>11</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>290</v>
       </c>
       <c r="H49">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I49">
-        <f>10*H49</f>
-        <v>140</v>
+        <f>10*H49*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>268</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>122</v>
+        <v>135</v>
+      </c>
+      <c r="B50" s="9">
+        <v>300</v>
       </c>
       <c r="C50" s="11">
         <v>805</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E50" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>284</v>
+        <v>11</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>292</v>
       </c>
       <c r="H50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50">
-        <f>10*H50</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C51" s="11">
         <v>805</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E51" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F51" t="s">
-        <v>19</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>285</v>
+        <v>11</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <f>10*H51</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>139</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C52" s="11">
         <v>805</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="F52" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I52">
-        <f>10*H52</f>
-        <v>30</v>
+        <f>10*H52*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="C53" s="11">
         <v>805</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E53" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="F53" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>287</v>
+        <v>11</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I53">
-        <f>10*H53</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C54" s="11">
         <v>805</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E54" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>288</v>
+        <v>11</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>294</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I54">
-        <f>10*H54</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="9">
-        <v>20</v>
+        <v>146</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="C55" s="11">
         <v>805</v>
       </c>
       <c r="D55" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E55" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="F55" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>289</v>
+        <v>11</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>295</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <f>10*H55</f>
-        <v>10</v>
+        <f>10*H55*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" s="11">
-        <v>805</v>
+        <v>151</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E56" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="F56" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>297</v>
+        <v>11</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <f>10*H56</f>
-        <v>10</v>
+        <f>10*H56*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="C57" s="11">
         <v>805</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E57" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="15" t="s">
-        <v>299</v>
+        <v>11</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57">
-        <f>10*H57</f>
-        <v>10</v>
+        <f>10*H57*2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>141</v>
-      </c>
-      <c r="B58" s="9">
-        <v>200</v>
-      </c>
-      <c r="C58" s="11">
-        <v>805</v>
+        <v>157</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="D58" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="E58" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="F58" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>298</v>
+        <v>11</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58">
-        <f>10*H58</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>143</v>
-      </c>
-      <c r="B59" s="9">
-        <v>300</v>
-      </c>
-      <c r="C59" s="11">
-        <v>805</v>
+        <v>159</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="F59" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>300</v>
+        <v>11</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59">
-        <f>10*H59</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>264</v>
+        <v>164</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C60" s="11">
-        <v>805</v>
+        <v>165</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>166</v>
       </c>
       <c r="D60" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="F60" t="s">
-        <v>19</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>301</v>
+        <v>11</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I60">
-        <f>10*H60</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61" s="11">
-        <v>805</v>
+        <v>169</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="D61" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="F61" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>291</v>
+        <v>11</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <f>10*H61</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>266</v>
+        <v>172</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" s="11">
-        <v>805</v>
+        <v>173</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="D62" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="E62" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="F62" t="s">
-        <v>19</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>290</v>
+        <v>11</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="H62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62">
-        <f>10*H62</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>267</v>
+        <v>176</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C63" s="11">
-        <v>805</v>
+        <v>177</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>178</v>
       </c>
       <c r="D63" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="E63" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="F63" t="s">
-        <v>19</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>302</v>
+        <v>11</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63">
-        <f>10*H63</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" t="s">
-        <v>154</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" s="11">
-        <v>805</v>
-      </c>
-      <c r="D64" t="s">
-        <v>118</v>
-      </c>
-      <c r="E64" t="s">
-        <v>156</v>
-      </c>
-      <c r="F64" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>303</v>
+      <c r="A64" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>307</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <f>10*H64</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="D65" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="F65" t="s">
-        <v>19</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>293</v>
+        <v>11</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="H65">
         <v>1</v>
       </c>
       <c r="I65">
-        <f>10*H65</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C66" s="11">
-        <v>805</v>
+        <v>188</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="D66" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="E66" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="F66" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>292</v>
+        <v>11</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>239</v>
       </c>
       <c r="H66">
         <v>1</v>
       </c>
       <c r="I66">
-        <f>10*H66</f>
+        <f t="shared" ref="I66:I97" si="2">10*H66</f>
         <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="B67" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" t="s">
+        <v>190</v>
+      </c>
+      <c r="E67" t="s">
+        <v>195</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C67" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D67" t="s">
-        <v>77</v>
-      </c>
-      <c r="E67" t="s">
-        <v>166</v>
-      </c>
-      <c r="F67" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="H67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <f>10*H67</f>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E68" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="F68" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H68">
         <v>1</v>
       </c>
       <c r="I68">
-        <f>10*H68</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>203</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="F69" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>233</v>
+        <v>11</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <f>10*H69</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" t="s">
-        <v>176</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="D70" t="s">
-        <v>170</v>
-      </c>
-      <c r="E70" t="s">
-        <v>179</v>
-      </c>
-      <c r="F70" t="s">
-        <v>19</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
+      <c r="A70" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H70" s="6">
+        <v>16</v>
       </c>
       <c r="I70">
-        <f>10*H70</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="J70" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>180</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>182</v>
+        <v>286</v>
+      </c>
+      <c r="B71" s="9">
+        <v>0</v>
+      </c>
+      <c r="C71" s="11">
+        <v>805</v>
       </c>
       <c r="D71" t="s">
-        <v>170</v>
-      </c>
-      <c r="E71" t="s">
-        <v>183</v>
-      </c>
-      <c r="F71" t="s">
-        <v>19</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>244</v>
+        <v>296</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>287</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I71">
-        <f>10*H71</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" t="s">
-        <v>184</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D72" t="s">
-        <v>170</v>
-      </c>
-      <c r="E72" t="s">
-        <v>187</v>
-      </c>
-      <c r="F72" t="s">
-        <v>19</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="I72">
-        <f>10*H72</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H73">
-        <v>4</v>
-      </c>
-      <c r="I73">
-        <f>10*H73</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" t="s">
-        <v>192</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D74" t="s">
-        <v>170</v>
-      </c>
-      <c r="E74" t="s">
-        <v>194</v>
-      </c>
-      <c r="F74" t="s">
-        <v>19</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74">
-        <f>10*H74</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>195</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="D75" t="s">
-        <v>198</v>
-      </c>
-      <c r="E75" t="s">
-        <v>199</v>
-      </c>
-      <c r="F75" t="s">
-        <v>19</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <f>10*H75</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" t="s">
-        <v>200</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" t="s">
-        <v>198</v>
-      </c>
-      <c r="E76" t="s">
-        <v>203</v>
-      </c>
-      <c r="F76" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <f>10*H76</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" t="s">
-        <v>204</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="D77" t="s">
-        <v>198</v>
-      </c>
-      <c r="E77" t="s">
-        <v>207</v>
-      </c>
-      <c r="F77" t="s">
-        <v>19</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="H77">
-        <v>1</v>
-      </c>
-      <c r="I77">
-        <f>10*H77</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" t="s">
-        <v>208</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D78" t="s">
-        <v>211</v>
-      </c>
-      <c r="E78" t="s">
-        <v>212</v>
-      </c>
-      <c r="F78" t="s">
-        <v>19</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78">
-        <f>10*H78</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H79" s="6">
-        <v>16</v>
-      </c>
-      <c r="I79">
-        <f>10*H79</f>
-        <v>160</v>
-      </c>
-      <c r="J79" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" t="s">
-        <v>294</v>
-      </c>
-      <c r="B80" s="9">
-        <v>0</v>
-      </c>
-      <c r="C80" s="11">
-        <v>805</v>
-      </c>
-      <c r="D80" t="s">
-        <v>304</v>
-      </c>
-      <c r="G80" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="H80">
-        <v>3</v>
-      </c>
-      <c r="I80">
-        <f>10*H80</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G80" r:id="rId1"/>
-    <hyperlink ref="G48" r:id="rId2"/>
-    <hyperlink ref="G56" r:id="rId3"/>
-    <hyperlink ref="G58" r:id="rId4"/>
-    <hyperlink ref="G57" r:id="rId5"/>
-    <hyperlink ref="G59" r:id="rId6"/>
-    <hyperlink ref="G60" r:id="rId7"/>
-    <hyperlink ref="G63" r:id="rId8"/>
-    <hyperlink ref="G64" r:id="rId9"/>
-    <hyperlink ref="G31" r:id="rId10"/>
-    <hyperlink ref="G17" r:id="rId11"/>
-    <hyperlink ref="G18" r:id="rId12"/>
-    <hyperlink ref="G27" r:id="rId13"/>
-    <hyperlink ref="G28" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
+    <hyperlink ref="G71" r:id="rId1"/>
+    <hyperlink ref="G39" r:id="rId2"/>
+    <hyperlink ref="G47" r:id="rId3"/>
+    <hyperlink ref="G49" r:id="rId4"/>
+    <hyperlink ref="G48" r:id="rId5"/>
+    <hyperlink ref="G50" r:id="rId6"/>
+    <hyperlink ref="G51" r:id="rId7"/>
+    <hyperlink ref="G54" r:id="rId8"/>
+    <hyperlink ref="G55" r:id="rId9"/>
+    <hyperlink ref="G22" r:id="rId10"/>
+    <hyperlink ref="G8" r:id="rId11"/>
+    <hyperlink ref="G9" r:id="rId12"/>
+    <hyperlink ref="G18" r:id="rId13"/>
+    <hyperlink ref="G19" r:id="rId14"/>
+    <hyperlink ref="G7" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
starting to change traces
</commit_message>
<xml_diff>
--- a/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
+++ b/hardware/gen5/MotherBoard/mother_Board_BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catodonnell/Documents/GitHub/robocup-ee/hardware/gen5/MotherBoard/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="-20" windowWidth="14400" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="460" windowWidth="14400" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,11 @@
   <definedNames>
     <definedName name="partlistKicker" localSheetId="0">Sheet1!$A$1:$F$69</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1171,6 +1179,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1503,10 +1516,10 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="9" bestFit="1" customWidth="1"/>
@@ -1516,7 +1529,7 @@
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1558,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1575,7 +1588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1605,7 +1618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1635,7 +1648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1665,7 +1678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1695,7 +1708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -1725,7 +1738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>246</v>
       </c>
@@ -1755,7 +1768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>265</v>
       </c>
@@ -1785,7 +1798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>250</v>
       </c>
@@ -1815,7 +1828,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>249</v>
       </c>
@@ -1845,7 +1858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>251</v>
       </c>
@@ -1875,7 +1888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1905,7 +1918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>248</v>
       </c>
@@ -1935,7 +1948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -1956,7 +1969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1986,7 +1999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2016,7 +2029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>252</v>
       </c>
@@ -2046,7 +2059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2076,7 +2089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2106,7 +2119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>227</v>
       </c>
@@ -2136,7 +2149,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2163,7 +2176,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2193,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2223,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -2253,7 +2266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>228</v>
       </c>
@@ -2283,7 +2296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2313,7 +2326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>80</v>
       </c>
@@ -2343,7 +2356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>226</v>
       </c>
@@ -2373,7 +2386,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>226</v>
       </c>
@@ -2403,7 +2416,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2430,7 +2443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>88</v>
       </c>
@@ -2458,7 +2471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
@@ -2484,7 +2497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>230</v>
       </c>
@@ -2511,7 +2524,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2541,7 +2554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -2568,7 +2581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -2598,7 +2611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>253</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2658,7 +2671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>254</v>
       </c>
@@ -2688,7 +2701,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>260</v>
       </c>
@@ -2718,7 +2731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>255</v>
       </c>
@@ -2748,7 +2761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>257</v>
       </c>
@@ -2778,7 +2791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>119</v>
       </c>
@@ -2804,11 +2817,11 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <f>10*H44*2</f>
+        <f t="shared" ref="I44:I49" si="2">10*H44*2</f>
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -2834,11 +2847,11 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f>10*H45*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -2864,11 +2877,11 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f>10*H46*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -2894,11 +2907,11 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <f>10*H47*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2924,11 +2937,11 @@
         <v>1</v>
       </c>
       <c r="I48">
-        <f>10*H48*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -2954,11 +2967,11 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f>10*H49*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -2988,7 +3001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>256</v>
       </c>
@@ -3018,7 +3031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>139</v>
       </c>
@@ -3048,7 +3061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>258</v>
       </c>
@@ -3078,7 +3091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>259</v>
       </c>
@@ -3108,7 +3121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>146</v>
       </c>
@@ -3138,7 +3151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>150</v>
       </c>
@@ -3168,7 +3181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -3198,7 +3211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>157</v>
       </c>
@@ -3228,7 +3241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>159</v>
       </c>
@@ -3258,7 +3271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>164</v>
       </c>
@@ -3288,7 +3301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>168</v>
       </c>
@@ -3318,7 +3331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>172</v>
       </c>
@@ -3348,7 +3361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>176</v>
       </c>
@@ -3378,7 +3391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>180</v>
       </c>
@@ -3408,7 +3421,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -3438,7 +3451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>187</v>
       </c>
@@ -3464,11 +3477,11 @@
         <v>1</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I97" si="2">10*H66</f>
+        <f t="shared" ref="I66:I71" si="3">10*H66</f>
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>192</v>
       </c>
@@ -3494,11 +3507,11 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>196</v>
       </c>
@@ -3524,11 +3537,11 @@
         <v>1</v>
       </c>
       <c r="I68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>200</v>
       </c>
@@ -3554,11 +3567,11 @@
         <v>1</v>
       </c>
       <c r="I69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>217</v>
       </c>
@@ -3574,14 +3587,14 @@
         <v>16</v>
       </c>
       <c r="I70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="J70" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>286</v>
       </c>
@@ -3601,7 +3614,7 @@
         <v>3</v>
       </c>
       <c r="I71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
@@ -3625,10 +3638,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>